<commit_message>
adidng excel file of the evaluation
</commit_message>
<xml_diff>
--- a/ML-Essay scoring/ClassificationResults.xlsx
+++ b/ML-Essay scoring/ClassificationResults.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\USERS-Load\PycharmProjects\pythonProject\ML-Essay scoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2681C85-82EA-4D2A-8440-1C34D6C11C26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55853E40-307D-47A8-8889-1BCC45FE0892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sbert results" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="91">
   <si>
     <t>Sbert Without Clusters</t>
   </si>
@@ -82,18 +82,6 @@
     <t>[[  0   0   0   8   0   0   0]</t>
   </si>
   <si>
-    <t xml:space="preserve"> [  0   0   0  65   0   0   0]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [  0   0   0 149   0   0   0]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [  0   0   0 235   0   0   0]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [  0   0   0  98   0   0   0]</t>
-  </si>
-  <si>
     <t xml:space="preserve"> [  0   0   0  16   0   0   0]</t>
   </si>
   <si>
@@ -127,27 +115,6 @@
     <t>Accuracy - LogisticRegression classifier</t>
   </si>
   <si>
-    <t>[[  2   3   2   1   0   0   0]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [  2   9  26  22   5   1   0]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [  2  26  45  58  14   4   0]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [  0  25  62 114  31   2   1]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [  0   4  19  46  24   5   0]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [  0   1   1  11   1   2   0]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [  0   0   0   0   2   0   0]]</t>
-  </si>
-  <si>
     <t xml:space="preserve">QWK between rater 1 and rater 2 is </t>
   </si>
   <si>
@@ -205,27 +172,6 @@
     <t xml:space="preserve"> [  0   0   0  14   1   1   0]</t>
   </si>
   <si>
-    <t>[[  0   0   7   1   0   0   0]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [  0   0  39  26   0   0   0]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [  0   2  79  68   0   0   0]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [  0   2 105 127   1   0   0]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [  0   1  28  67   2   0   0]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [  0   0   4  11   1   0   0]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [  0   0   1   1   0   0   0]]</t>
-  </si>
-  <si>
     <t>Accuracy - DecisionTree classifier - depth  =5</t>
   </si>
   <si>
@@ -253,16 +199,106 @@
     <t xml:space="preserve"> [  0   0   0  15   1   0   0]</t>
   </si>
   <si>
-    <t>Accuracy - SVC - C = 0.025</t>
-  </si>
-  <si>
-    <t>Accuracy - SVC - C = 1</t>
-  </si>
-  <si>
-    <t>Accuracy - SVC  - C = 0.025</t>
-  </si>
-  <si>
     <t>tfIDF with Clusters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pearson correlation </t>
+  </si>
+  <si>
+    <t>(0.0848, 0.0424)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adjecent accuracy </t>
+  </si>
+  <si>
+    <t>(0.187, 6.594e-06)</t>
+  </si>
+  <si>
+    <t>(0.2024, 1.022e-06)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [  0   0  20  43   2   0   0]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [  0   0  40 103   6   0   0]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [  0   0  39 187   9   0   0]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [  0   0  11  81   6   0   0]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [  0   0   0   1   1   0   0]]</t>
+  </si>
+  <si>
+    <t>(0.2675, 7.579e-11)</t>
+  </si>
+  <si>
+    <t>(0.21004, 3.899e-07)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accuracy - SVC </t>
+  </si>
+  <si>
+    <t>(0.2748, 2.154e-11)</t>
+  </si>
+  <si>
+    <t>[[  0   0   2   6   0   0   0]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [  0   0  11  54   0   0   0]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [  0   0  15 134   0   0   0]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [  0   0   8 227   0   0   0]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [  0   0   3  95   0   0   0]</t>
+  </si>
+  <si>
+    <t>(0.229, 2.66e-08)</t>
+  </si>
+  <si>
+    <t>(0.22, 4.464e-08)</t>
+  </si>
+  <si>
+    <t>(0.191, 3.7005e-06)</t>
+  </si>
+  <si>
+    <t>Accuracy - SVC</t>
+  </si>
+  <si>
+    <t>(0.22644792460094076, 4.251198903046183e-08)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (0.2685690644036752, 6.350139877975657e-11)</t>
+  </si>
+  <si>
+    <t>(0.24563573741579806, 2.54447850065474e-09)</t>
+  </si>
+  <si>
+    <t>[[ 1  2  2  3  0  0  0]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [ 2 13 32 14  3  1  0]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [ 2 31 54 41 16  5  0]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [ 0 43 76 74 39  2  1]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [ 0 13 22 30 29  4  0]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [ 0  0  3  9  2  2  0]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [ 0  0  0  1  1  0  0]]</t>
   </si>
 </sst>
 </file>
@@ -624,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -637,7 +673,7 @@
     <col min="8" max="8" width="33.21875" customWidth="1"/>
     <col min="9" max="9" width="43.44140625" customWidth="1"/>
     <col min="10" max="10" width="24.88671875" customWidth="1"/>
-    <col min="11" max="11" width="15.88671875" customWidth="1"/>
+    <col min="11" max="11" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
@@ -647,7 +683,7 @@
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="D1" s="1" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>8</v>
@@ -657,10 +693,10 @@
       </c>
       <c r="G1" s="3"/>
       <c r="H1" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>8</v>
@@ -709,21 +745,45 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D5" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="E5" t="s">
         <v>4</v>
       </c>
+      <c r="F5" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="G5" s="3"/>
+      <c r="I5" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="J5" t="s">
-        <v>24</v>
+        <v>20</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>77</v>
+      </c>
       <c r="E6" t="s">
         <v>5</v>
       </c>
+      <c r="F6">
+        <v>0.86212914485165704</v>
+      </c>
       <c r="G6" s="3"/>
+      <c r="I6" t="s">
+        <v>81</v>
+      </c>
       <c r="J6" t="s">
         <v>5</v>
+      </c>
+      <c r="K6">
+        <v>0.86212914485165704</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -771,7 +831,7 @@
       </c>
       <c r="G10" s="3"/>
       <c r="I10" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>8</v>
@@ -795,7 +855,7 @@
         <v>0.34031413612565398</v>
       </c>
       <c r="J11" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="K11">
         <v>0.26850570861650103</v>
@@ -807,7 +867,7 @@
       </c>
       <c r="G12" s="3"/>
       <c r="J12" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
@@ -816,25 +876,49 @@
       </c>
       <c r="G13" s="3"/>
       <c r="J13" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D14" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="E14" t="s">
         <v>14</v>
       </c>
+      <c r="F14" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="G14" s="3"/>
+      <c r="I14" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="J14" t="s">
-        <v>28</v>
+        <v>24</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
+        <v>78</v>
+      </c>
       <c r="E15" t="s">
         <v>15</v>
       </c>
+      <c r="F15">
+        <v>0.83944153577661396</v>
+      </c>
       <c r="G15" s="3"/>
+      <c r="I15" t="s">
+        <v>82</v>
+      </c>
       <c r="J15" t="s">
-        <v>29</v>
+        <v>25</v>
+      </c>
+      <c r="K15">
+        <v>0.78708551483420597</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
@@ -843,7 +927,7 @@
       </c>
       <c r="G16" s="3"/>
       <c r="J16" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
@@ -852,7 +936,7 @@
       </c>
       <c r="G17" s="3"/>
       <c r="J17" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
@@ -871,7 +955,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D19" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>8</v>
@@ -881,7 +965,7 @@
       </c>
       <c r="G19" s="3"/>
       <c r="I19" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>8</v>
@@ -892,20 +976,20 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D20">
-        <v>0.41012216404886498</v>
+        <v>0.42233856893542698</v>
       </c>
       <c r="E20" t="s">
-        <v>17</v>
+        <v>72</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>8.4556038281358603E-2</v>
       </c>
       <c r="G20" s="3"/>
       <c r="I20">
-        <v>0.34205933682373402</v>
+        <v>0.30191972076788798</v>
       </c>
       <c r="J20" t="s">
-        <v>33</v>
+        <v>84</v>
       </c>
       <c r="K20">
         <v>0.286961672036111</v>
@@ -913,47 +997,71 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E21" t="s">
-        <v>18</v>
+        <v>73</v>
       </c>
       <c r="G21" s="3"/>
       <c r="J21" t="s">
-        <v>34</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E22" t="s">
-        <v>19</v>
+        <v>74</v>
       </c>
       <c r="G22" s="3"/>
       <c r="J22" t="s">
-        <v>35</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D23" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="E23" t="s">
-        <v>20</v>
+        <v>75</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="G23" s="3"/>
+      <c r="I23" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="J23" t="s">
-        <v>36</v>
+        <v>87</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D24" t="s">
+        <v>79</v>
+      </c>
       <c r="E24" t="s">
-        <v>21</v>
+        <v>76</v>
+      </c>
+      <c r="F24">
+        <v>0.85514834205933599</v>
       </c>
       <c r="G24" s="3"/>
+      <c r="I24" t="s">
+        <v>83</v>
+      </c>
       <c r="J24" t="s">
-        <v>37</v>
+        <v>88</v>
+      </c>
+      <c r="K24">
+        <v>0.75392670157067998</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E25" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G25" s="3"/>
       <c r="J25" t="s">
-        <v>38</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
@@ -962,7 +1070,7 @@
       </c>
       <c r="G26" s="3"/>
       <c r="J26" t="s">
-        <v>39</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
@@ -981,7 +1089,7 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F29" s="5" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="G29">
         <v>0.39773002428690202</v>
@@ -997,8 +1105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92CFF813-41C7-4BF7-855B-214EDFD46B3B}">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1015,12 +1123,12 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="D1" s="1" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>8</v>
@@ -1030,10 +1138,10 @@
       </c>
       <c r="G1" s="3"/>
       <c r="H1" s="4" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>8</v>
@@ -1054,58 +1162,82 @@
       </c>
       <c r="G2" s="3"/>
       <c r="I2">
-        <v>0.363001745200698</v>
+        <v>0.35951134380453698</v>
       </c>
       <c r="J2" t="s">
-        <v>59</v>
+        <v>17</v>
       </c>
       <c r="K2">
-        <v>0.16835260434358701</v>
+        <v>4.2608962240049099E-2</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E3" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="G3" s="3"/>
       <c r="J3" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E4" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="G4" s="3"/>
       <c r="J4" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D5" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="E5" t="s">
-        <v>50</v>
+        <v>39</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="G5" s="3"/>
+      <c r="I5" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="J5" t="s">
-        <v>62</v>
+        <v>39</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>59</v>
+      </c>
       <c r="E6" t="s">
-        <v>51</v>
+        <v>40</v>
+      </c>
+      <c r="F6">
+        <v>0.84816753926701505</v>
       </c>
       <c r="G6" s="3"/>
+      <c r="I6" t="s">
+        <v>69</v>
+      </c>
       <c r="J6" t="s">
-        <v>63</v>
+        <v>40</v>
+      </c>
+      <c r="K6">
+        <v>0.85514834205933599</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E7" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="G7" s="3"/>
       <c r="J7" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
@@ -1114,7 +1246,7 @@
       </c>
       <c r="G8" s="3"/>
       <c r="J8" t="s">
-        <v>65</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
@@ -1144,7 +1276,7 @@
       </c>
       <c r="G10" s="3"/>
       <c r="I10" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>8</v>
@@ -1158,17 +1290,19 @@
         <v>0.39616055846422299</v>
       </c>
       <c r="E11" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="F11">
-        <v>0.145600349135344</v>
-      </c>
-      <c r="G11" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="G11" s="3">
+        <v>1</v>
+      </c>
       <c r="I11">
         <v>0.37521815008726001</v>
       </c>
       <c r="J11" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="K11">
         <v>0.24176168929110101</v>
@@ -1176,47 +1310,71 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E12" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="G12" s="3"/>
       <c r="J12" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E13" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="G13" s="3"/>
       <c r="J13" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D14" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="E14" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G14" s="3"/>
+      <c r="I14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J14" t="s">
         <v>45</v>
       </c>
-      <c r="G14" s="3"/>
-      <c r="J14" t="s">
-        <v>56</v>
+      <c r="K14" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
+        <v>61</v>
+      </c>
       <c r="E15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15">
+        <v>0.84293193717277404</v>
+      </c>
+      <c r="G15" s="3"/>
+      <c r="I15" t="s">
+        <v>68</v>
+      </c>
+      <c r="J15" t="s">
         <v>46</v>
       </c>
-      <c r="G15" s="3"/>
-      <c r="J15" t="s">
-        <v>57</v>
+      <c r="K15">
+        <v>0.85165794066317602</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E16" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="G16" s="3"/>
       <c r="J16" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
@@ -1244,7 +1402,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D19" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>8</v>
@@ -1254,7 +1412,7 @@
       </c>
       <c r="G19" s="3"/>
       <c r="I19" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>8</v>
@@ -1265,20 +1423,20 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D20">
-        <v>0.41012216404886498</v>
+        <v>0.40663176265270501</v>
       </c>
       <c r="E20" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>0.14987146409625901</v>
       </c>
       <c r="G20" s="3"/>
       <c r="I20">
         <v>0.38568935427574103</v>
       </c>
       <c r="J20" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="K20">
         <v>0.22858711327405001</v>
@@ -1286,52 +1444,76 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E21" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
       <c r="G21" s="3"/>
       <c r="J21" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D22" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="E22" t="s">
-        <v>19</v>
+        <v>64</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="G22" s="3"/>
+      <c r="I22" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="J22" t="s">
+        <v>53</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D23" t="s">
+        <v>62</v>
+      </c>
+      <c r="E23" t="s">
+        <v>65</v>
+      </c>
+      <c r="F23">
+        <v>0.84816753926701505</v>
+      </c>
+      <c r="G23" s="3"/>
+      <c r="I23" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E23" t="s">
-        <v>20</v>
-      </c>
-      <c r="G23" s="3"/>
       <c r="J23" t="s">
-        <v>72</v>
+        <v>54</v>
+      </c>
+      <c r="K23">
+        <v>0.86561954624781801</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E24" t="s">
-        <v>21</v>
+        <v>66</v>
       </c>
       <c r="G24" s="3"/>
       <c r="J24" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E25" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="G25" s="3"/>
       <c r="J25" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E26" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
       <c r="G26" s="3"/>
       <c r="J26" t="s">
@@ -1354,7 +1536,7 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F29" s="5" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="G29">
         <v>0.39773002428690202</v>

</xml_diff>